<commit_message>
feat: add vocabularies with legend description
</commit_message>
<xml_diff>
--- a/mentor-dashboard/src/rawSource/Mentor-students pairs.xlsx
+++ b/mentor-dashboard/src/rawSource/Mentor-students pairs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1308">
   <si>
     <t>Name</t>
   </si>
@@ -3939,6 +3939,9 @@
   </si>
   <si>
     <t>fdf</t>
+  </si>
+  <si>
+    <t>Aliaksei KRAUCHANKA</t>
   </si>
 </sst>
 </file>
@@ -4373,8 +4376,8 @@
   </sheetPr>
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5306,7 +5309,7 @@
     </row>
     <row r="116" spans="1:2" ht="15.75" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>219</v>
+        <v>1307</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>225</v>

</xml_diff>

<commit_message>
feat: merge mentorScore data
</commit_message>
<xml_diff>
--- a/mentor-dashboard/src/rawSource/Mentor-students pairs.xlsx
+++ b/mentor-dashboard/src/rawSource/Mentor-students pairs.xlsx
@@ -11,14 +11,14 @@
     <sheet name="second_name-to_github_account" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pairs!$A$1:$A$997</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">pairs!$A$1:$A$996</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="1306">
   <si>
     <t>Name</t>
   </si>
@@ -3933,12 +3933,6 @@
   </si>
   <si>
     <t>seidou99</t>
-  </si>
-  <si>
-    <t>Petya Bockin</t>
-  </si>
-  <si>
-    <t>fdf</t>
   </si>
   <si>
     <t>Aliaksei KRAUCHANKA</t>
@@ -4374,10 +4368,10 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D997"/>
+  <dimension ref="A1:D996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A117" sqref="A117"/>
+    <sheetView tabSelected="1" topLeftCell="A778" workbookViewId="0">
+      <selection activeCell="B1003" sqref="B1003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -5309,7 +5303,7 @@
     </row>
     <row r="116" spans="1:2" ht="15.75" customHeight="1">
       <c r="A116" s="2" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>225</v>
@@ -10689,21 +10683,17 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="787" spans="1:2" ht="15.75" customHeight="1">
+    <row r="787" spans="1:2" ht="23.25" customHeight="1">
       <c r="A787" s="2" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="788" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A788" s="2" t="s">
-        <v>1299</v>
-      </c>
-      <c r="B788" s="2" t="s">
         <v>1304</v>
       </c>
+    </row>
+    <row r="788" spans="1:2" ht="15.75" hidden="1" customHeight="1">
+      <c r="A788" s="2"/>
+      <c r="B788" s="2"/>
     </row>
     <row r="789" spans="1:2" ht="15.75" hidden="1" customHeight="1">
       <c r="A789" s="2"/>
@@ -10721,10 +10711,7 @@
       <c r="A792" s="2"/>
       <c r="B792" s="2"/>
     </row>
-    <row r="793" spans="1:2" ht="15.75" hidden="1" customHeight="1">
-      <c r="A793" s="2"/>
-      <c r="B793" s="2"/>
-    </row>
+    <row r="793" spans="1:2" ht="15.75" hidden="1" customHeight="1"/>
     <row r="794" spans="1:2" ht="15.75" hidden="1" customHeight="1"/>
     <row r="795" spans="1:2" ht="15.75" hidden="1" customHeight="1"/>
     <row r="796" spans="1:2" ht="15.75" hidden="1" customHeight="1"/>
@@ -10928,9 +10915,8 @@
     <row r="994" ht="15.75" hidden="1" customHeight="1"/>
     <row r="995" ht="15.75" hidden="1" customHeight="1"/>
     <row r="996" ht="15.75" hidden="1" customHeight="1"/>
-    <row r="997" ht="15.75" hidden="1" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:A997">
+  <autoFilter ref="A1:A996">
     <filterColumn colId="0">
       <customFilters and="1">
         <customFilter operator="notEqual" val=" "/>

</xml_diff>

<commit_message>
refactor: change dir to components
</commit_message>
<xml_diff>
--- a/mentor-dashboard/src/rawSource/Mentor-students pairs.xlsx
+++ b/mentor-dashboard/src/rawSource/Mentor-students pairs.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="1306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="1307">
   <si>
     <t>Name</t>
   </si>
@@ -3936,6 +3936,9 @@
   </si>
   <si>
     <t>Aliaksei KRAUCHANKA</t>
+  </si>
+  <si>
+    <t>Rem  Apasov</t>
   </si>
 </sst>
 </file>
@@ -4370,8 +4373,8 @@
   </sheetPr>
   <dimension ref="A1:D996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A778" workbookViewId="0">
-      <selection activeCell="B1003" sqref="B1003"/>
+    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
+      <selection activeCell="A590" sqref="A590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -9117,7 +9120,7 @@
     </row>
     <row r="591" spans="1:2" ht="15.75" customHeight="1">
       <c r="A591" s="2" t="s">
-        <v>68</v>
+        <v>1306</v>
       </c>
       <c r="B591" s="2" t="s">
         <v>1071</v>
@@ -10936,8 +10939,8 @@
   </sheetPr>
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat: merge mentor name and city to out json
</commit_message>
<xml_diff>
--- a/mentor-dashboard/src/rawSource/Mentor-students pairs.xlsx
+++ b/mentor-dashboard/src/rawSource/Mentor-students pairs.xlsx
@@ -4373,8 +4373,8 @@
   </sheetPr>
   <dimension ref="A1:D996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A570" workbookViewId="0">
-      <selection activeCell="A590" sqref="A590"/>
+    <sheetView tabSelected="1" topLeftCell="A772" workbookViewId="0">
+      <selection activeCell="A1003" sqref="A1003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>